<commit_message>
successfully created functionality to create randomised lists and randomised sub groups of any size
</commit_message>
<xml_diff>
--- a/randomised_list.xlsx
+++ b/randomised_list.xlsx
@@ -7,7 +7,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet 0" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -15,24 +14,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+  <si>
+    <t>Group 1</t>
+  </si>
+  <si>
+    <t>Group 2</t>
+  </si>
+  <si>
+    <t>Group 3</t>
+  </si>
+  <si>
+    <t>world</t>
+  </si>
+  <si>
+    <t>are</t>
+  </si>
+  <si>
+    <t>how</t>
+  </si>
+  <si>
+    <t>you</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
   <si>
     <t>today</t>
-  </si>
-  <si>
-    <t>hello</t>
-  </si>
-  <si>
-    <t>you</t>
-  </si>
-  <si>
-    <t>are</t>
-  </si>
-  <si>
-    <t>how</t>
-  </si>
-  <si>
-    <t>world</t>
   </si>
 </sst>
 </file>
@@ -368,63 +376,246 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A1:A10"/>
+      <selection activeCell="E28" sqref="A1:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
 </file>
</xml_diff>